<commit_message>
Se agrego un nuevo campo a la tabla factura
</commit_message>
<xml_diff>
--- a/Sexto Trimestre/Diccionario De Datos.xlsx
+++ b/Sexto Trimestre/Diccionario De Datos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="4830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="97">
   <si>
     <t>Factura</t>
   </si>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>Campo que guarda la identificacion de la persona</t>
-  </si>
-  <si>
-    <t>Campo que guarda el ide la sucursal</t>
   </si>
   <si>
     <t>Campo que guarda el id del tipo del producto</t>
@@ -475,7 +472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -514,9 +511,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -533,6 +527,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -844,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,25 +896,25 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -916,7 +943,7 @@
     <row r="5" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -932,7 +959,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -976,160 +1003,154 @@
     <row r="8" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="B9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="29"/>
     </row>
     <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="E15" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1138,13 +1159,13 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>13</v>
@@ -1156,151 +1177,153 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="56.25" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>20</v>
@@ -1312,383 +1335,381 @@
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="25"/>
+    </row>
+    <row r="36" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="3" t="s">
+    <row r="37" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3" t="s">
+      <c r="D37" s="3"/>
+      <c r="E37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3" t="s">
+    <row r="38" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="25"/>
+    </row>
+    <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="B44" s="9" t="s">
-        <v>78</v>
+      <c r="B44" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="3"/>
       <c r="F44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H44" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="E45" s="3"/>
       <c r="F45" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B46" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="B47" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
+      <c r="B47" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="22"/>
+    </row>
+    <row r="50" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="25"/>
+    </row>
+    <row r="51" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H52" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -1697,140 +1718,140 @@
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
+      <c r="B55" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="56" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
-      <c r="B56" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
     </row>
     <row r="58" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="22"/>
+    </row>
+    <row r="59" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="25"/>
+    </row>
+    <row r="60" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-      <c r="B59" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D61" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G61" s="3"/>
+      <c r="G61" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H61" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -1845,30 +1866,28 @@
     <row r="63" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D63" s="3"/>
-      <c r="E63" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="E63" s="3"/>
       <c r="F63" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -1877,530 +1896,560 @@
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B65" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
+      <c r="B66" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="67" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
-      <c r="B67" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
     </row>
     <row r="69" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="22"/>
+    </row>
+    <row r="70" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="25"/>
+    </row>
+    <row r="71" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="H71" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D71" s="3"/>
-      <c r="E71" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="D72" s="3"/>
-      <c r="E72" s="12"/>
+      <c r="E72" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F72" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="56.25" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D73" s="3"/>
-      <c r="E73" s="12"/>
+      <c r="E73" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="F73" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-    </row>
-    <row r="75" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B74" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
+      <c r="B75" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="76" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
-      <c r="B76" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
     </row>
     <row r="78" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="22"/>
+    </row>
+    <row r="79" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="25"/>
+    </row>
+    <row r="80" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H80" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H79" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D81" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="10"/>
-      <c r="H81" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G81" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B82" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
+      <c r="B83" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G83" s="10"/>
+      <c r="H83" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="84" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
-      <c r="B84" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
     </row>
     <row r="85" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
     </row>
     <row r="86" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="21"/>
+      <c r="H86" s="22"/>
+    </row>
+    <row r="87" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="25"/>
+    </row>
+    <row r="88" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E88" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="H88" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C87" s="3" t="s">
+    <row r="89" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="B89" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D89" s="3"/>
+      <c r="D89" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G89" s="10"/>
-      <c r="H89" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B90" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C90" s="9" t="s">
+      <c r="G89" s="3"/>
+      <c r="H89" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="9"/>
-      <c r="H90" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3" t="s">
+      <c r="G91" s="10"/>
+      <c r="H91" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B92" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="5"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="14"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="14"/>
+    <row r="94" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
     </row>
     <row r="96" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" s="21"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="22"/>
+    </row>
+    <row r="97" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="23"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="25"/>
+    </row>
+    <row r="98" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E98" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="H98" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="2:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B97" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C97" s="3" t="s">
+    <row r="99" spans="2:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B99" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B98" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C98" s="3" t="s">
+      <c r="D99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B100" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G98" s="10"/>
-      <c r="H98" s="3" t="s">
-        <v>84</v>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G100" s="10"/>
+      <c r="H100" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B94:H95"/>
+  <mergeCells count="1">
     <mergeCell ref="B2:H3"/>
-    <mergeCell ref="B10:H11"/>
-    <mergeCell ref="B21:H22"/>
-    <mergeCell ref="B56:H57"/>
-    <mergeCell ref="B67:H68"/>
-    <mergeCell ref="B84:H85"/>
-    <mergeCell ref="B76:H77"/>
-    <mergeCell ref="B32:H33"/>
-    <mergeCell ref="B39:H40"/>
-    <mergeCell ref="B47:H48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1" location="Id_Factura" display="F:\Diccionario_De_Datos.html - Id_Factura"/>
-    <hyperlink ref="E14" r:id="rId2" location="Referencia_Productos" display="F:\Diccionario_De_Datos.html - Referencia_Productos"/>
-    <hyperlink ref="E35" r:id="rId3" location="Persona_Identificacion" display="F:\Diccionario_De_Datos.html - Persona_Identificacion"/>
-    <hyperlink ref="E36" r:id="rId4" location="Id_Sucursal" display="F:\Diccionario_De_Datos.html - Id_Sucursal"/>
-    <hyperlink ref="E63" r:id="rId5" location="NIT_Restaurante" display="F:\Diccionario_De_Datos.html - NIT_Restaurante"/>
-    <hyperlink ref="E70" r:id="rId6" location="Id_Sucursal" display="F:\Diccionario_De_Datos.html - Id_Sucursal"/>
-    <hyperlink ref="E71" r:id="rId7" location="Referencia_Productos" display="F:\Diccionario_De_Datos.html - Referencia_Productos"/>
+    <hyperlink ref="E15" r:id="rId1" location="Id_Factura" display="F:\Diccionario_De_Datos.html - Id_Factura"/>
+    <hyperlink ref="E16" r:id="rId2" location="Referencia_Productos" display="F:\Diccionario_De_Datos.html - Referencia_Productos"/>
+    <hyperlink ref="E37" r:id="rId3" location="Persona_Identificacion" display="F:\Diccionario_De_Datos.html - Persona_Identificacion"/>
+    <hyperlink ref="E38" r:id="rId4" location="Id_Sucursal" display="F:\Diccionario_De_Datos.html - Id_Sucursal"/>
+    <hyperlink ref="E65" r:id="rId5" location="NIT_Restaurante" display="F:\Diccionario_De_Datos.html - NIT_Restaurante"/>
+    <hyperlink ref="E72" r:id="rId6" location="Id_Sucursal" display="F:\Diccionario_De_Datos.html - Id_Sucursal"/>
+    <hyperlink ref="E73" r:id="rId7" location="Referencia_Productos" display="F:\Diccionario_De_Datos.html - Referencia_Productos"/>
     <hyperlink ref="E7" r:id="rId8" location="Persona_Identificacion" display="F:\Diccionario_De_Datos.html - Persona_Identificacion"/>
-    <hyperlink ref="E45" r:id="rId9" location="Id_TipoProductos" display="F:\Diccionario_De_Datos.html - Id_TipoProductos"/>
+    <hyperlink ref="E47" r:id="rId9" location="Id_TipoProductos" display="F:\Diccionario_De_Datos.html - Id_TipoProductos"/>
+    <hyperlink ref="E8" r:id="rId10" location="Id_Sucursal" display="F:\Diccionario_De_Datos.html - Id_Sucursal"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>